<commit_message>
Recommsys ver. 0.3.1 (normalization)
</commit_message>
<xml_diff>
--- a/migforecasting/clustering/recommendation system/for medians.xlsx
+++ b/migforecasting/clustering/recommendation system/for medians.xlsx
@@ -517,7 +517,7 @@
   <dimension ref="A1:AJ8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -679,9 +679,8 @@
         <f t="shared" si="0"/>
         <v>1.8671553542408596E-3</v>
       </c>
-      <c r="L3" s="7">
-        <f t="shared" si="0"/>
-        <v>1.5442066318592027E-2</v>
+      <c r="L3" s="8">
+        <v>446.6</v>
       </c>
       <c r="M3" s="7">
         <f t="shared" si="0"/>
@@ -696,8 +695,7 @@
         <v>94.265330147643581</v>
       </c>
       <c r="P3" s="7">
-        <f t="shared" si="0"/>
-        <v>1.0373085301338093E-3</v>
+        <v>29.999999999999901</v>
       </c>
       <c r="Q3" s="7">
         <f t="shared" si="0"/>
@@ -775,7 +773,7 @@
         <v>19876.724880000002</v>
       </c>
       <c r="F4" s="7">
-        <f t="shared" ref="E4:F8" si="4">Y4/$C4</f>
+        <f t="shared" ref="F4:F8" si="4">Y4/$C4</f>
         <v>0.57319900555041337</v>
       </c>
       <c r="G4" s="7">
@@ -797,9 +795,8 @@
         <f t="shared" si="0"/>
         <v>2.3993987049028649E-3</v>
       </c>
-      <c r="L4" s="7">
-        <f t="shared" si="0"/>
-        <v>1.4809782608695624E-2</v>
+      <c r="L4" s="8">
+        <v>512.29999999999905</v>
       </c>
       <c r="M4" s="7">
         <f t="shared" si="0"/>
@@ -814,8 +811,7 @@
         <v>100.22669981498584</v>
       </c>
       <c r="P4" s="7">
-        <f t="shared" si="0"/>
-        <v>1.0696114708603145E-3</v>
+        <v>37</v>
       </c>
       <c r="Q4" s="7">
         <f t="shared" si="0"/>
@@ -915,9 +911,8 @@
         <f t="shared" si="0"/>
         <v>2.7916406737367437E-3</v>
       </c>
-      <c r="L5" s="7">
-        <f t="shared" si="0"/>
-        <v>6.0527136618839517E-3</v>
+      <c r="L5" s="8">
+        <v>388.099999999999</v>
       </c>
       <c r="M5" s="7">
         <f t="shared" si="0"/>
@@ -932,8 +927,7 @@
         <v>8.7406379772301772</v>
       </c>
       <c r="P5" s="7">
-        <f t="shared" si="0"/>
-        <v>4.5227698066125857E-4</v>
+        <v>28.999999999999901</v>
       </c>
       <c r="Q5" s="7">
         <f t="shared" si="0"/>
@@ -1033,9 +1027,8 @@
         <f t="shared" si="0"/>
         <v>1.9904845130595248E-3</v>
       </c>
-      <c r="L6" s="7">
-        <f t="shared" si="0"/>
-        <v>1.8967860957374544E-2</v>
+      <c r="L6" s="8">
+        <v>390.69999999999902</v>
       </c>
       <c r="M6" s="7">
         <f t="shared" si="0"/>
@@ -1050,8 +1043,7 @@
         <v>86.713398674628536</v>
       </c>
       <c r="P6" s="7">
-        <f t="shared" si="0"/>
-        <v>1.3108068744538367E-3</v>
+        <v>27</v>
       </c>
       <c r="Q6" s="7">
         <f t="shared" si="0"/>
@@ -1151,9 +1143,8 @@
         <f t="shared" si="0"/>
         <v>2.6976951011635632E-3</v>
       </c>
-      <c r="L7" s="7">
-        <f t="shared" si="0"/>
-        <v>7.4334840287556218E-3</v>
+      <c r="L7" s="8">
+        <v>250.74999999999901</v>
       </c>
       <c r="M7" s="7">
         <f t="shared" si="0"/>
@@ -1168,8 +1159,7 @@
         <v>7.0141793878306977</v>
       </c>
       <c r="P7" s="7">
-        <f t="shared" si="0"/>
-        <v>4.1503001556362557E-4</v>
+        <v>14</v>
       </c>
       <c r="Q7" s="7">
         <f t="shared" si="0"/>
@@ -1269,9 +1259,8 @@
         <f t="shared" si="0"/>
         <v>1.9707669568073656E-3</v>
       </c>
-      <c r="L8" s="7">
-        <f t="shared" si="0"/>
-        <v>2.2778781409098479E-2</v>
+      <c r="L8" s="8">
+        <v>277.39999999999901</v>
       </c>
       <c r="M8" s="7">
         <f t="shared" si="0"/>
@@ -1286,8 +1275,7 @@
         <v>38.35219197733641</v>
       </c>
       <c r="P8" s="7">
-        <f t="shared" si="0"/>
-        <v>1.3138446378715743E-3</v>
+        <v>15.999999999999901</v>
       </c>
       <c r="Q8" s="7">
         <f t="shared" si="0"/>
@@ -1348,7 +1336,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3:B8">
-    <cfRule type="colorScale" priority="42">
+    <cfRule type="colorScale" priority="44">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -1360,6 +1348,126 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W3:W8">
+    <cfRule type="colorScale" priority="26">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="X3:X8">
+    <cfRule type="colorScale" priority="29">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB3:AB8">
+    <cfRule type="colorScale" priority="30">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AC3:AC8">
+    <cfRule type="colorScale" priority="31">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE3:AE8">
+    <cfRule type="colorScale" priority="32">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AG3:AG8">
+    <cfRule type="colorScale" priority="33">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AI3:AI8">
+    <cfRule type="colorScale" priority="34">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AH3:AH8">
+    <cfRule type="colorScale" priority="28">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AF3:AF8">
+    <cfRule type="colorScale" priority="27">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Y3:Y8">
+    <cfRule type="colorScale" priority="25">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA3:AA8">
     <cfRule type="colorScale" priority="24">
       <colorScale>
         <cfvo type="min"/>
@@ -1371,103 +1479,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="X3:X8">
-    <cfRule type="colorScale" priority="27">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AB3:AB8">
-    <cfRule type="colorScale" priority="28">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AC3:AC8">
-    <cfRule type="colorScale" priority="29">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AE3:AE8">
-    <cfRule type="colorScale" priority="30">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AG3:AG8">
-    <cfRule type="colorScale" priority="31">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AI3:AI8">
-    <cfRule type="colorScale" priority="32">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AH3:AH8">
-    <cfRule type="colorScale" priority="26">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AF3:AF8">
-    <cfRule type="colorScale" priority="25">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Y3:Y8">
+  <conditionalFormatting sqref="Z3:Z8">
     <cfRule type="colorScale" priority="23">
       <colorScale>
         <cfvo type="min"/>
@@ -1479,7 +1491,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA3:AA8">
+  <conditionalFormatting sqref="AD3:AD8">
     <cfRule type="colorScale" priority="22">
       <colorScale>
         <cfvo type="min"/>
@@ -1491,7 +1503,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z3:Z8">
+  <conditionalFormatting sqref="AJ3:AJ8">
     <cfRule type="colorScale" priority="21">
       <colorScale>
         <cfvo type="min"/>
@@ -1503,19 +1515,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AD3:AD8">
-    <cfRule type="colorScale" priority="20">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AJ3:AJ8">
+  <conditionalFormatting sqref="C3:C8">
     <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="min"/>
@@ -1527,19 +1527,19 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C3:C8">
-    <cfRule type="colorScale" priority="17">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="D3:D8">
+    <cfRule type="colorScale" priority="18">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F3:F8">
     <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="min"/>
@@ -1551,7 +1551,19 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F3:F8">
+  <conditionalFormatting sqref="G3:G8">
+    <cfRule type="colorScale" priority="15">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3:E8">
     <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
@@ -1563,7 +1575,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G3:G8">
+  <conditionalFormatting sqref="H3:H8">
     <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min"/>
@@ -1575,19 +1587,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E3:E8">
-    <cfRule type="colorScale" priority="12">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H3:H8">
+  <conditionalFormatting sqref="J3:J8">
     <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min"/>
@@ -1599,19 +1599,19 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J3:J8">
-    <cfRule type="colorScale" priority="9">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="K3:K8">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M3:M8">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
@@ -1623,79 +1623,67 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="N3:N8">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O3:O8">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q3:Q8">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I3:I8">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P3:P8">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="L3:L8">
-    <cfRule type="colorScale" priority="7">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M3:M8">
-    <cfRule type="colorScale" priority="6">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N3:N8">
-    <cfRule type="colorScale" priority="5">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O3:O8">
-    <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P3:P8">
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Q3:Q8">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I3:I8">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>